<commit_message>
Update Intersection Over Union.xlsx
</commit_message>
<xml_diff>
--- a/Intersection Over Union/Intersection Over Union.xlsx
+++ b/Intersection Over Union/Intersection Over Union.xlsx
@@ -9857,8 +9857,8 @@
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="C66" s="1">
-        <v>132.0</v>
+      <c r="C66" s="3">
+        <v>381.0</v>
       </c>
       <c r="D66" s="1">
         <v>728.0</v>
@@ -9871,7 +9871,7 @@
       </c>
       <c r="G66" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;taggedRectangle x="132" y="728" width="412" height="8" offset="0"  /&gt;</v>
+        <v>&lt;taggedRectangle x="381" y="728" width="163" height="8" offset="0"  /&gt;</v>
       </c>
     </row>
     <row r="67">

</xml_diff>